<commit_message>
Export inc a total souboru
</commit_message>
<xml_diff>
--- a/MetricsAPI/Metriky/ObecnyPomer.xlsx
+++ b/MetricsAPI/Metriky/ObecnyPomer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hapes\Downloads\Metriky\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hapes\source\repos\MetricsAPI\MetricsAPI\Metriky\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F11FB99-FBCE-4F47-B440-95BEF8301CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447DCF9E-1F3C-471E-969F-D1FBD82A6555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4965" yWindow="5190" windowWidth="21600" windowHeight="11385" xr2:uid="{ABB27848-C041-4BE9-9E5F-AA33F99E07E4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ABB27848-C041-4BE9-9E5F-AA33F99E07E4}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Datum</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Pocet pribytku celkem</t>
+  </si>
+  <si>
+    <t>Release</t>
   </si>
 </sst>
 </file>
@@ -398,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB6FFC68-F0C6-4270-B4A1-46DCF8C365E5}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,7 +414,7 @@
     <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -421,8 +424,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44876</v>
       </c>
@@ -432,8 +438,11 @@
       <c r="C2">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44877</v>
       </c>
@@ -443,8 +452,11 @@
       <c r="C3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44878</v>
       </c>
@@ -454,8 +466,11 @@
       <c r="C4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44879</v>
       </c>
@@ -465,8 +480,11 @@
       <c r="C5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44880</v>
       </c>
@@ -476,8 +494,11 @@
       <c r="C6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44881</v>
       </c>
@@ -487,8 +508,11 @@
       <c r="C7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44882</v>
       </c>
@@ -498,8 +522,11 @@
       <c r="C8">
         <v>200</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44883</v>
       </c>
@@ -509,8 +536,11 @@
       <c r="C9">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44884</v>
       </c>
@@ -520,8 +550,11 @@
       <c r="C10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44885</v>
       </c>
@@ -530,6 +563,9 @@
       </c>
       <c r="C11">
         <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>